<commit_message>
aanvulling wat is twitter, verwijzing in titels naar titelbar en TODO
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicole\Documents\GitHub\Twitter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laura\Documents\GitHub\Twitter\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>TODO</t>
   </si>
@@ -141,7 +141,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,6 +151,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -182,10 +188,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -279,6 +286,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -314,6 +338,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -468,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,6 +544,10 @@
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B3" s="3"/>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -582,7 +627,7 @@
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -608,6 +653,7 @@
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="B24" s="3"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">

</xml_diff>

<commit_message>
TODO, sitemap, kleuren en div css
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
   <si>
     <t>TODO</t>
   </si>
@@ -111,6 +111,18 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Laura/nicole</t>
+  </si>
+  <si>
+    <t>nicole/Laura</t>
+  </si>
+  <si>
+    <t>in geschiedenis</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -509,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,11 +565,17 @@
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -571,31 +589,50 @@
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E9" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="D10" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="D11" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="D12" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="B13" s="3"/>
       <c r="D13" s="1" t="s">
         <v>27</v>
       </c>
@@ -604,16 +641,23 @@
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="D14" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="D16" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="C17" s="3"/>
       <c r="D17" s="1" t="s">
         <v>27</v>
       </c>
@@ -622,6 +666,10 @@
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -638,6 +686,10 @@
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -648,21 +700,33 @@
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="D23" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="D25" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>26</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
flot, in map, TODO, grafiek, eerste tekst incl refs en contactgegevens
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -153,7 +153,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -169,6 +169,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -200,11 +206,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -521,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,7 +563,7 @@
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
       <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
@@ -649,6 +656,7 @@
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="C16" s="4"/>
       <c r="D16" s="1" t="s">
         <v>30</v>
       </c>
@@ -700,6 +708,7 @@
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="C23" s="3"/>
       <c r="D23" s="1" t="s">
         <v>9</v>
       </c>

</xml_diff>